<commit_message>
Improvement with one table.  Looks like need parent/child Feature/Dependency.
</commit_message>
<xml_diff>
--- a/fmmdemo/FMM.xlsx
+++ b/fmmdemo/FMM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e352454\dev\Projects\fmmdemo\fmmdemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E310F1AA-7512-4B27-BD6B-E07105E4741C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0191BF00-DAF3-4386-8EE7-343D129414BB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FMM" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="FMM" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId4"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="420">
   <si>
     <t>Installation</t>
   </si>
@@ -1278,12 +1282,15 @@
   </si>
   <si>
     <t>Function_Name from Shell</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1781,7 +1788,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1792,6 +1799,7 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1848,6 +1856,2847 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Cottle, Rick (CS CoE)" refreshedDate="43244.366873495368" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="149" xr:uid="{8CFABAEC-8843-4C21-9AC7-09FD39949295}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:H150" sheet="FMM"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Group" numFmtId="0">
+      <sharedItems count="12">
+        <s v="Electrical Power"/>
+        <s v="Air Cooled ECU"/>
+        <s v="Aircraft Interfaces"/>
+        <s v="Communications"/>
+        <s v="Environmental"/>
+        <s v="Turbo Prop"/>
+        <s v="Monitoring"/>
+        <s v="Turbo Fan"/>
+        <s v="Engine Power"/>
+        <s v="Installation"/>
+        <s v="Fuel Cooled ECU"/>
+        <s v="Engine Speed"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Function" numFmtId="0">
+      <sharedItems count="88">
+        <s v="Aircraft Power"/>
+        <s v="Anti-Ice Coil"/>
+        <s v="Anti-Ice Command Switch"/>
+        <s v="ARINC-429 Configuration"/>
+        <s v="Audio Frequency Conducted Susceptibility"/>
+        <s v="Avionics Data Bus"/>
+        <s v="Beta Pressure Sensor"/>
+        <s v="Chip Detector Connection"/>
+        <s v="Compressor Guide Vanes (CGV) LVDT"/>
+        <s v="Condition Lever"/>
+        <s v="Cross Engine Data Link"/>
+        <s v="Drivers and Torque Motor Wiring"/>
+        <s v="ECO Mode"/>
+        <s v="ECU Enclosure Type"/>
+        <s v="Electrical Grounding"/>
+        <s v="Engine Count"/>
+        <s v="Engine Cutoff Indication"/>
+        <s v="Engine Discrete Electrical Interface"/>
+        <s v="Engine ID"/>
+        <s v="Engine Idle Switch"/>
+        <s v="Engine Speed Analog Output"/>
+        <s v="Engine Type"/>
+        <s v="Engine Wiring Configuration"/>
+        <s v="Ethernet"/>
+        <s v="Exhaust Gas Temperature"/>
+        <s v="Feather Coil"/>
+        <s v="Filter Inlet Static Pressure Selection"/>
+        <s v="Filter Inlet Static Pressure Type"/>
+        <s v="Filter Type Available"/>
+        <s v="Final PLA Adjustment"/>
+        <s v="Flight Idle Switch"/>
+        <s v="Fuel Filter Bypass Connection"/>
+        <s v="Fuel Filter Bypass Indication"/>
+        <s v="Fuel Temperature Sensor"/>
+        <s v="Ground Idle Switch"/>
+        <s v="GSE Interface"/>
+        <s v="Igniter A and B High Side Driver"/>
+        <s v="Ignition Switch"/>
+        <s v="Inlet Static Pressure Location"/>
+        <s v="Low Oil Level Indicator"/>
+        <s v="Mach Hold"/>
+        <s v="Maintenance Enabled Switch"/>
+        <s v="Manual Power Reserve"/>
+        <s v="Metering Valve"/>
+        <s v="Motive Flow Lockout Coil"/>
+        <s v="Muted Recovery Degraded Mode "/>
+        <s v="N1"/>
+        <s v="NTS Oil Pressure Sensor"/>
+        <s v="Oil Filter Bypass Connection"/>
+        <s v="Oil Filter Bypass Indication"/>
+        <s v="Oil Pressure Sensor Type"/>
+        <s v="Oil Temperature Sensor"/>
+        <s v="Output Driver Selection"/>
+        <s v="Overspeed Coil"/>
+        <s v="P3 Sensor Installation"/>
+        <s v="PCU Reset Switch"/>
+        <s v="PLA Difference Fault Signal Selection"/>
+        <s v="PLA Dual Fault Signal Selection"/>
+        <s v="PLA Input"/>
+        <s v="PLA Selection"/>
+        <s v="PLA Single Fault Signal Selection"/>
+        <s v="PLA Takeoff Limitation"/>
+        <s v="PMA Power"/>
+        <s v="Power Demand"/>
+        <s v="Propeller Governor"/>
+        <s v="Propeller Pitch Control"/>
+        <s v="Propeller Pitch Controller"/>
+        <s v="Radio Frequency Conducted Emissions"/>
+        <s v="Radio Frequency Conducted Susceptibility"/>
+        <s v="Reset Degraded Mode "/>
+        <s v="Reverse Request Switch"/>
+        <s v="Run Coil"/>
+        <s v="Scavenge De-Oil Coil"/>
+        <s v="Secondary N2"/>
+        <s v="Shutdown Switch"/>
+        <s v="Speed"/>
+        <s v="Start Command Switch"/>
+        <s v="Starter Relay"/>
+        <s v="Supply De-Oil Coil"/>
+        <s v="Synchrophasing"/>
+        <s v="Throttle Control"/>
+        <s v="Torque Sensor"/>
+        <s v="TT2 Temperature"/>
+        <s v="Turboprop Spare"/>
+        <s v="Unfeather Pump"/>
+        <s v="Vibration Output for GSE"/>
+        <s v="Vibration Sensor"/>
+        <s v="Weight-on-wheels Switch"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Feature_Name" numFmtId="0">
+      <sharedItems count="135">
+        <s v="Single Aircraft Power Source"/>
+        <s v="Dual Aircraft Power Source"/>
+        <s v="Anti-Ice Coil Installed"/>
+        <s v="Anti-Ice Command SW Installed"/>
+        <s v="Independent Engine Wiring A/I Command"/>
+        <s v="Shared Engine Wiring A/I Command"/>
+        <s v="Dual ARINC-429"/>
+        <s v="Quad ARINC-429"/>
+        <s v="DO-160 Audio Frequency Conducted Susceptibility Requirements"/>
+        <s v="MIL-STD-461 Audio Frequency Conducted Susceptibility Requirements"/>
+        <s v="ARINC-429"/>
+        <s v="MIL-STD-1553"/>
+        <s v="Available"/>
+        <s v="Shared Channel"/>
+        <s v="Single Channel Input"/>
+        <s v="CGV LVDT"/>
+        <s v="Condition Lever Installed"/>
+        <s v="Cross Engine Data Link"/>
+        <s v="Drivers and Torque Motor Wiring for Air Cooled Application"/>
+        <s v="ECO Mode"/>
+        <s v="Air Cooled"/>
+        <s v="Fuel Cooled"/>
+        <s v="Common-Ground System"/>
+        <s v="Isolated-Ground System"/>
+        <s v="Single Engine"/>
+        <s v="Dual Engines"/>
+        <s v="Engine Cutoff Indication Input"/>
+        <s v="Right Engine ID Valid Configuration"/>
+        <s v="Engine Idle Switch installed"/>
+        <s v="N2 Speed Analog Output"/>
+        <s v="N1 Speed Analog Output"/>
+        <s v="Turbo Prop"/>
+        <s v="Turbo Fan"/>
+        <s v="Independent Engine Wiring"/>
+        <s v="Shared Engine Wiring"/>
+        <s v="Ethernet data streaming capability"/>
+        <s v="Ethernet data dump capability"/>
+        <s v="EGT 4 Thermocouple"/>
+        <s v="EGT 3 Thermocouple"/>
+        <s v="Feather Coil Installed"/>
+        <s v="Raw Static Pressure Unfiltered"/>
+        <s v="Raw Static Pressure Filtered"/>
+        <s v="Filter using Self-Adjusting Time Constant Filter"/>
+        <s v="Self-Adjusting Time Constant Filter for analog inputs"/>
+        <s v="Final PLA adjusted with Autothrottle trim"/>
+        <s v="Final PLA"/>
+        <s v="Flight Idle SW Installed"/>
+        <s v="Independent Engine Wiring FI"/>
+        <s v="Shared Engine Wiring FI"/>
+        <s v="Closed Circuit Indicates Bypass"/>
+        <s v="Open Circuit Indicates Bypass"/>
+        <s v="Installed"/>
+        <s v="Ground Idle SW Installed"/>
+        <s v="Independent Engine Wiring GI"/>
+        <s v="Shared Engine Wiring GI"/>
+        <s v="Has Ethernet transmit capability"/>
+        <s v="RS-422 Only"/>
+        <s v="Igniter A and B High Side Driver Installed"/>
+        <s v="Ignition SW Installed"/>
+        <s v="Independent Engine Wiring Ign"/>
+        <s v="Shared Engine Wiring Ign"/>
+        <s v="Inlet Static Pressure is measured at a plumbed location"/>
+        <s v="Inlet Static Pressure is measured internally in ECU"/>
+        <s v="Mach Hold Mode Enabled"/>
+        <s v="Independent Engine Wiring Mach Hold"/>
+        <s v="Shared Engine Wiring Mach Hold"/>
+        <s v="Maintenance Enabled SW Installed"/>
+        <s v="Independent Engine Wiring Maint"/>
+        <s v="Shared Engine Wiring Maint"/>
+        <s v="Manual Power Reserve Discrete (MPR) option"/>
+        <s v="Manual Power Reserve Throttle Lever (MPR) option"/>
+        <s v="Metering Valve Torque Motor Installed"/>
+        <s v="Motive Flow Lockout Coil Installed"/>
+        <s v="Has muted recovery for degraded mode"/>
+        <s v="Has N1"/>
+        <s v="Dual Transducer Pressure Sensor; Single Channel Inputs"/>
+        <s v="Single Transducer Pressure Sensor; Single Channel Inputs"/>
+        <s v="Not Installed"/>
+        <s v="Output Driver Selection for Dual Channel"/>
+        <s v="Overspeed Coil Installed"/>
+        <s v="External P3 sensors each plumbed to a single ECU Channel"/>
+        <s v="ECU Internal P3 sensors each plumbed to a single ECU Channel"/>
+        <s v="PCU Reset Switch Installed"/>
+        <s v="PLA Difference Fault Fail to Idle"/>
+        <s v="PLA Difference Fault choose High between LC &amp; XC PLA"/>
+        <s v="PLA Dual Fault set Degrade Mode 2"/>
+        <s v="PLA Dual Fault Fail to Default Value"/>
+        <s v="PLA via Arinc"/>
+        <s v="PLA via Analog"/>
+        <s v="PLA selection can be overridden by the Idle Discrete Switch"/>
+        <s v="PLA selection standard "/>
+        <s v="PLA Single Fault choose remaining Healthy plus Offset"/>
+        <s v="PLA Single Fault choose remaining Healthy"/>
+        <s v="Engine Power Rating Limited by Altitude"/>
+        <s v="Engine Power Rating not Limited by Altitude"/>
+        <s v="PMA Power Source"/>
+        <s v="Power Demand Reverse to MPR Selection"/>
+        <s v="Power Demand Idle to Max Selection"/>
+        <s v="Propeller Governor Torque Motor Installed"/>
+        <s v="PPC RVDT Installation"/>
+        <s v="Propeller Pitch Controller Installed"/>
+        <s v="DO-160 Radio Frequency Conducted Emissions Requirements"/>
+        <s v="MIL-STD-461 Radio Frequency Conducted Emissions Requirements"/>
+        <s v="DO-160 Radio Frequency Conducted Susceptibility Requirements"/>
+        <s v="MIL-STD-461 Radio Frequency Conducted Susceptibility Requirements"/>
+        <s v="Has reset enable for degraded mode"/>
+        <s v="Reverse Request SW Installed"/>
+        <s v="Independent Engine Wiring RR"/>
+        <s v="Shared Engine Wiring RR"/>
+        <s v="Run Coil Installed"/>
+        <s v="Scavenge De-Oil Coil Installed"/>
+        <s v="Has Secondary N2"/>
+        <s v="No Secondary N2"/>
+        <s v="Shutdown SW Installed"/>
+        <s v="Independent Engine Wiring Shutdown"/>
+        <s v="Shared Engine Wiring Shutdown"/>
+        <s v="N1"/>
+        <s v="N2 Twin Spool"/>
+        <s v="N2 Single Spool"/>
+        <s v="Start Command SW Installed"/>
+        <s v="Independent Engine Wiring Start"/>
+        <s v="Shared Engine Wiring Start"/>
+        <s v="Starter Relay Installed"/>
+        <s v="Supply De-Oil Coil Installed"/>
+        <s v="TurboProp Syncrophasing"/>
+        <s v="TurboFan Syncrophasing"/>
+        <s v="Autothrottle Installed"/>
+        <s v="3 Wire TT2"/>
+        <s v="2 Wire TT2"/>
+        <s v="Spare accounted for in Turboprop application"/>
+        <s v="Unfeather Pump Installed"/>
+        <s v="Vibration Output for GSE interface installed"/>
+        <s v="WOW SW Installed"/>
+        <s v="Independent Engine Wiring WOW"/>
+        <s v="Shared Engine Wiring WOW"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Feature" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Dependency" numFmtId="0">
+      <sharedItems count="40">
+        <s v="n/a"/>
+        <s v="airCooled"/>
+        <s v="aiCmdSW;indepEngineWiring"/>
+        <s v="aiCmdSW;sharedEngineWiring"/>
+        <s v="Arinc"/>
+        <s v="turboProp"/>
+        <s v="turboFan"/>
+        <s v="dualEngine"/>
+        <s v="fuelCooled"/>
+        <s v="afterBurner"/>
+        <s v="gseEthernet"/>
+        <s v="filterSelfAdjusting"/>
+        <s v="filterSelfAdjusting;psFiltered"/>
+        <s v="autoThrottle"/>
+        <s v="flightIdleSW;indepEngineWiring"/>
+        <s v="flightIdleSW;sharedEngineWiring"/>
+        <s v="engDisSharedElectInt"/>
+        <s v="engDis1ChanInputElectInt"/>
+        <s v="groundIdleSW;indepEngineWiring"/>
+        <s v="groundIdleSW;sharedEngineWiring"/>
+        <s v="ignitionSW;indepEngineWiring"/>
+        <s v="ignitionSW;sharedEngineWiring"/>
+        <s v="machHold;indepEngineWiring"/>
+        <s v="machHold;sharedEngineWiring"/>
+        <s v="maintEnableSW;indepEngineWiring"/>
+        <s v="maintEnableSW;sharedEngineWiring"/>
+        <s v="n1Common"/>
+        <s v="plaDiffFailedIdle"/>
+        <s v="plaDiffChooseHigh"/>
+        <s v="engineIdleDiscrete"/>
+        <s v="revRqstSW;indepEngineWiring"/>
+        <s v="revRqstSW;sharedEngineWiring"/>
+        <s v="shutdownSW;indepEngineWiring"/>
+        <s v="shutdownSW;sharedEngineWiring"/>
+        <s v="startCmdSW;indepEngineWiring"/>
+        <s v="startCmdSW;sharedEngineWiring"/>
+        <s v="turboProp;dualEngine"/>
+        <s v="turboFan;dualEngine"/>
+        <s v="wowSW;indepEngineWiring"/>
+        <s v="wowSW;sharedEngineWiring"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Rule" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Min" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Max" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="2"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="149">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="singleACPwr"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="dualACPwr"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="antiIceCoil"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="aiCmdSW"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <s v="aiCmdSingleEngineWiring"/>
+    <x v="2"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="5"/>
+    <s v="aiCmdDualEngineWiring"/>
+    <x v="3"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="6"/>
+    <s v="dualArinc"/>
+    <x v="4"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="7"/>
+    <s v="quadArinc"/>
+    <x v="4"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="8"/>
+    <s v="do160AFCS"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="9"/>
+    <s v="mil461AFCS"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="10"/>
+    <s v="Arinc"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="11"/>
+    <s v="Mil1553"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="12"/>
+    <s v="betaPressSensor"/>
+    <x v="5"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="7"/>
+    <x v="13"/>
+    <s v="chipDetectDualChSharedInput "/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="7"/>
+    <x v="14"/>
+    <s v="chipDetectSingleChInput"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="8"/>
+    <x v="15"/>
+    <s v="cgvLVDT"/>
+    <x v="6"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="9"/>
+    <x v="16"/>
+    <s v="conditionLever"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="10"/>
+    <x v="17"/>
+    <s v="xEngDataLink"/>
+    <x v="7"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="18"/>
+    <s v="DTMWiringAC"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="12"/>
+    <x v="19"/>
+    <s v="ecoMode"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="20"/>
+    <s v="airCooled"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="21"/>
+    <s v="fuelCooled"/>
+    <x v="6"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="14"/>
+    <x v="22"/>
+    <s v="commonGnd"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="14"/>
+    <x v="23"/>
+    <s v="isolatedGnd"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="15"/>
+    <x v="24"/>
+    <s v="singleEngine"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="15"/>
+    <x v="25"/>
+    <s v="dualEngine"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="16"/>
+    <x v="26"/>
+    <s v="engineCutoffind"/>
+    <x v="8"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="17"/>
+    <x v="13"/>
+    <s v="engDisSharedElectInt"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="17"/>
+    <x v="14"/>
+    <s v="engDis1ChanInputElectInt"/>
+    <x v="8"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="18"/>
+    <x v="27"/>
+    <s v="rightEngID"/>
+    <x v="7"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="19"/>
+    <x v="28"/>
+    <s v="engineIdleDiscrete"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="20"/>
+    <x v="29"/>
+    <s v="n2SpeedOutput"/>
+    <x v="5"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="20"/>
+    <x v="30"/>
+    <s v="n1SpeedOutput"/>
+    <x v="6"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="21"/>
+    <x v="31"/>
+    <s v="turboProp"/>
+    <x v="9"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="21"/>
+    <x v="32"/>
+    <s v="turboFan"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="22"/>
+    <x v="33"/>
+    <s v="indepEngineWiring"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="22"/>
+    <x v="34"/>
+    <s v="sharedEngineWiring"/>
+    <x v="7"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="23"/>
+    <x v="35"/>
+    <s v="gseEthernetDataStream"/>
+    <x v="10"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="23"/>
+    <x v="36"/>
+    <s v="gseEthernetDataDump"/>
+    <x v="10"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="24"/>
+    <x v="37"/>
+    <s v="egt4TC"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="24"/>
+    <x v="38"/>
+    <s v="egt3TC"/>
+    <x v="6"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="25"/>
+    <x v="39"/>
+    <s v="featherCoil"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="26"/>
+    <x v="40"/>
+    <s v="psUnfiltered"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="26"/>
+    <x v="41"/>
+    <s v="psFiltered"/>
+    <x v="11"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="27"/>
+    <x v="42"/>
+    <s v="psSelfAdjustingFiltered"/>
+    <x v="12"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="28"/>
+    <x v="43"/>
+    <s v="filterSelfAdjusting"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="29"/>
+    <x v="44"/>
+    <s v="plaFinalAdjustedAutoThrottle"/>
+    <x v="13"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="29"/>
+    <x v="45"/>
+    <s v="plaFinalAdjusted"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="30"/>
+    <x v="46"/>
+    <s v="flightIdleSW"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="30"/>
+    <x v="47"/>
+    <s v="flightIdleSingleEngineWiring"/>
+    <x v="14"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="30"/>
+    <x v="48"/>
+    <s v="flightIdleDualEngineWiring"/>
+    <x v="15"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="31"/>
+    <x v="13"/>
+    <s v="wfFiltBypSharedElectInt"/>
+    <x v="16"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="31"/>
+    <x v="14"/>
+    <s v="singleChannelInputWfFiltByp"/>
+    <x v="17"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="32"/>
+    <x v="49"/>
+    <s v="wfFiltBypClsdIsBypass"/>
+    <x v="8"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="32"/>
+    <x v="50"/>
+    <s v="wfFiltBypOpenIsBypass"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="33"/>
+    <x v="51"/>
+    <s v="fuelTempSensorAvail"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="34"/>
+    <x v="52"/>
+    <s v="groundIdleSW"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="34"/>
+    <x v="53"/>
+    <s v="groundIdleSingleEngineWiring"/>
+    <x v="18"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="34"/>
+    <x v="54"/>
+    <s v="groundIdleDualEngineWiring"/>
+    <x v="19"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="35"/>
+    <x v="55"/>
+    <s v="gseEthernet"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="35"/>
+    <x v="56"/>
+    <s v="gseRS422Only"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="36"/>
+    <x v="57"/>
+    <s v="HSIgniter"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="37"/>
+    <x v="58"/>
+    <s v="ignitionSW"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="37"/>
+    <x v="59"/>
+    <s v="ignitSingleEngineWiring"/>
+    <x v="20"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="37"/>
+    <x v="60"/>
+    <s v="ignitDualEngineWiring"/>
+    <x v="21"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="38"/>
+    <x v="61"/>
+    <s v="psPlumbed"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="38"/>
+    <x v="62"/>
+    <s v="psUnplumbed"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="39"/>
+    <x v="12"/>
+    <s v="singleChannelInputLOLAvail"/>
+    <x v="8"/>
+    <s v="Selection"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="40"/>
+    <x v="63"/>
+    <s v="machHold"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="40"/>
+    <x v="64"/>
+    <s v="machHoldSingleEngineWiring"/>
+    <x v="22"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="40"/>
+    <x v="65"/>
+    <s v="machHoldDualEngineWiring"/>
+    <x v="23"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="41"/>
+    <x v="66"/>
+    <s v="maintEnableSW"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="41"/>
+    <x v="67"/>
+    <s v="maintSingleEngineWiring"/>
+    <x v="24"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="41"/>
+    <x v="68"/>
+    <s v="maintDualEngineWiring"/>
+    <x v="25"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="42"/>
+    <x v="69"/>
+    <s v="powerRatingMPRDiscrete"/>
+    <x v="1"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="42"/>
+    <x v="70"/>
+    <s v="powerRatingMPRPushThrough"/>
+    <x v="1"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="43"/>
+    <x v="71"/>
+    <s v="meteringValve"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="44"/>
+    <x v="72"/>
+    <s v="motiveFlowLockoutCoil"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="45"/>
+    <x v="73"/>
+    <s v="ccdlDegradeLatch"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="46"/>
+    <x v="74"/>
+    <s v="n1Common"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="46"/>
+    <x v="74"/>
+    <s v="n1SingleSource"/>
+    <x v="26"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="47"/>
+    <x v="12"/>
+    <s v="ntsOilPressSensor"/>
+    <x v="5"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="48"/>
+    <x v="13"/>
+    <s v="oilFiltBypSharedElectInt"/>
+    <x v="16"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="48"/>
+    <x v="14"/>
+    <s v="singleChannelInputOilFiltByp"/>
+    <x v="17"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="49"/>
+    <x v="49"/>
+    <s v="oilFiltBypClsdIsBypass"/>
+    <x v="8"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="49"/>
+    <x v="50"/>
+    <s v="oilFiltBypOpenIsBypass"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="50"/>
+    <x v="75"/>
+    <s v="pSnsrDualXDCRSingleChanIn"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="50"/>
+    <x v="76"/>
+    <s v="pSnsrSingleXDCRSingleChanIn"/>
+    <x v="8"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="51"/>
+    <x v="51"/>
+    <s v="oilTempSensorAvail"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="51"/>
+    <x v="77"/>
+    <s v="oilTempSensorNotAvail"/>
+    <x v="8"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="52"/>
+    <x v="78"/>
+    <s v="ODSDualChannel"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="53"/>
+    <x v="79"/>
+    <s v="overspeedCoil"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="54"/>
+    <x v="80"/>
+    <s v="p3ExternalSeparatePipes "/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="54"/>
+    <x v="81"/>
+    <s v="p3InternalSeperatePipes"/>
+    <x v="8"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="55"/>
+    <x v="82"/>
+    <s v="pcuReset"/>
+    <x v="8"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="56"/>
+    <x v="83"/>
+    <s v="plaDiffFailedIdle"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="56"/>
+    <x v="84"/>
+    <s v="plaDiffChooseHigh"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="57"/>
+    <x v="85"/>
+    <s v="plaBothFaultedDG2"/>
+    <x v="27"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="57"/>
+    <x v="86"/>
+    <s v="plaBothFaultedDV"/>
+    <x v="28"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="58"/>
+    <x v="87"/>
+    <s v="thrustViaArinc"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="58"/>
+    <x v="88"/>
+    <s v="thrustViaDiscrete"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="59"/>
+    <x v="89"/>
+    <s v="plaPrimSelectIdleSW"/>
+    <x v="29"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="59"/>
+    <x v="90"/>
+    <s v="plaPrimSelectStandard"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="60"/>
+    <x v="91"/>
+    <s v="plaOffsetHealthy"/>
+    <x v="27"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="60"/>
+    <x v="92"/>
+    <s v="plaChooseHealthy"/>
+    <x v="28"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="61"/>
+    <x v="93"/>
+    <s v="plaTakeoffLimitation"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="61"/>
+    <x v="94"/>
+    <s v="plaTakeoffUnrestricted"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="62"/>
+    <x v="95"/>
+    <s v="pmaPower"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="63"/>
+    <x v="96"/>
+    <s v="plaRevMpr"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="63"/>
+    <x v="97"/>
+    <s v="plaIdleMax"/>
+    <x v="8"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="64"/>
+    <x v="98"/>
+    <s v="propGovernor"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="65"/>
+    <x v="99"/>
+    <s v="ppcVDT"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="66"/>
+    <x v="100"/>
+    <s v="propPitchController"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="67"/>
+    <x v="101"/>
+    <s v="do160RFCE"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="67"/>
+    <x v="102"/>
+    <s v="mil461RFCE"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="68"/>
+    <x v="103"/>
+    <s v="do160RFCS"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="68"/>
+    <x v="104"/>
+    <s v="mil461RFCS"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="69"/>
+    <x v="105"/>
+    <s v="ccdlDegradeBypass"/>
+    <x v="8"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="70"/>
+    <x v="106"/>
+    <s v="revRqstSW"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="70"/>
+    <x v="107"/>
+    <s v="revRqstSingleEngineWiring"/>
+    <x v="30"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="70"/>
+    <x v="108"/>
+    <s v="revRqstDualEngineWiring"/>
+    <x v="31"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="71"/>
+    <x v="109"/>
+    <s v="runCoil"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="72"/>
+    <x v="110"/>
+    <s v="scavengeDeOilCoil"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="73"/>
+    <x v="111"/>
+    <s v="n2SecondarySource"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="73"/>
+    <x v="112"/>
+    <s v="n2SingleSource"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="74"/>
+    <x v="113"/>
+    <s v="shutdownSW"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="74"/>
+    <x v="114"/>
+    <s v="shutdownSingleEngineWiring"/>
+    <x v="32"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="74"/>
+    <x v="115"/>
+    <s v="shutdownDualEngineWiring"/>
+    <x v="33"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="75"/>
+    <x v="116"/>
+    <s v="n1speed"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="75"/>
+    <x v="117"/>
+    <s v="n2Twin"/>
+    <x v="0"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="75"/>
+    <x v="118"/>
+    <s v="n2Single"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="76"/>
+    <x v="119"/>
+    <s v="startCmdSW"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="76"/>
+    <x v="120"/>
+    <s v="startCmdSingleEngineWiring"/>
+    <x v="34"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="76"/>
+    <x v="121"/>
+    <s v="startCmdDualEngineWiring"/>
+    <x v="35"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="77"/>
+    <x v="122"/>
+    <s v="starterRelay"/>
+    <x v="1"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="78"/>
+    <x v="123"/>
+    <s v="supplyDeOilCoil"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="79"/>
+    <x v="124"/>
+    <s v="propSyncrophase"/>
+    <x v="36"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="79"/>
+    <x v="125"/>
+    <s v="fanSyncrophase"/>
+    <x v="37"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="80"/>
+    <x v="126"/>
+    <s v="autoThrottle"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="81"/>
+    <x v="12"/>
+    <s v="torqueSensor"/>
+    <x v="5"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="82"/>
+    <x v="127"/>
+    <s v="tt2ThreeWire"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="82"/>
+    <x v="128"/>
+    <s v="tt2TwoWire"/>
+    <x v="6"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="83"/>
+    <x v="129"/>
+    <s v="spareTurboProp"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="84"/>
+    <x v="130"/>
+    <s v="unfeatherPump"/>
+    <x v="5"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="85"/>
+    <x v="131"/>
+    <s v="vibrationOutput"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="86"/>
+    <x v="51"/>
+    <s v="vibrationSense"/>
+    <x v="1"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="87"/>
+    <x v="132"/>
+    <s v="wowSW"/>
+    <x v="0"/>
+    <s v="Option"/>
+    <n v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="87"/>
+    <x v="133"/>
+    <s v="wowSingleEngineWiring"/>
+    <x v="38"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="87"/>
+    <x v="134"/>
+    <s v="wowDualEngineWiring"/>
+    <x v="39"/>
+    <s v="Selection"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BE9039C4-BE7E-4385-A46F-68BA8F4F3E5C}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:J154" firstHeaderRow="2" firstDataRow="2" firstDataCol="4"/>
+  <pivotFields count="8">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="12">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="88">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="135">
+        <item x="128"/>
+        <item x="127"/>
+        <item x="20"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="126"/>
+        <item x="12"/>
+        <item x="15"/>
+        <item x="49"/>
+        <item x="22"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="8"/>
+        <item x="101"/>
+        <item x="103"/>
+        <item x="18"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="25"/>
+        <item x="75"/>
+        <item x="19"/>
+        <item x="81"/>
+        <item x="38"/>
+        <item x="37"/>
+        <item x="26"/>
+        <item x="28"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="36"/>
+        <item x="35"/>
+        <item x="80"/>
+        <item x="39"/>
+        <item x="42"/>
+        <item x="45"/>
+        <item x="44"/>
+        <item x="46"/>
+        <item x="21"/>
+        <item x="52"/>
+        <item x="55"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="105"/>
+        <item x="111"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="33"/>
+        <item x="4"/>
+        <item x="47"/>
+        <item x="53"/>
+        <item x="59"/>
+        <item x="64"/>
+        <item x="67"/>
+        <item x="107"/>
+        <item x="114"/>
+        <item x="120"/>
+        <item x="133"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="51"/>
+        <item x="23"/>
+        <item x="63"/>
+        <item x="66"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="11"/>
+        <item x="9"/>
+        <item x="102"/>
+        <item x="104"/>
+        <item x="72"/>
+        <item x="116"/>
+        <item x="30"/>
+        <item x="118"/>
+        <item x="29"/>
+        <item x="117"/>
+        <item x="112"/>
+        <item x="77"/>
+        <item x="50"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="82"/>
+        <item x="84"/>
+        <item x="83"/>
+        <item x="86"/>
+        <item x="85"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="92"/>
+        <item x="91"/>
+        <item x="88"/>
+        <item x="87"/>
+        <item x="95"/>
+        <item x="97"/>
+        <item x="96"/>
+        <item x="99"/>
+        <item x="98"/>
+        <item x="100"/>
+        <item x="7"/>
+        <item x="41"/>
+        <item x="40"/>
+        <item x="106"/>
+        <item x="27"/>
+        <item x="56"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="43"/>
+        <item x="13"/>
+        <item x="34"/>
+        <item x="5"/>
+        <item x="48"/>
+        <item x="54"/>
+        <item x="60"/>
+        <item x="65"/>
+        <item x="68"/>
+        <item x="108"/>
+        <item x="115"/>
+        <item x="121"/>
+        <item x="134"/>
+        <item x="113"/>
+        <item x="0"/>
+        <item x="14"/>
+        <item x="24"/>
+        <item x="76"/>
+        <item x="129"/>
+        <item x="119"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="32"/>
+        <item x="31"/>
+        <item x="125"/>
+        <item x="124"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="41">
+        <item x="9"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="7"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="29"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="8"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="10"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="0"/>
+        <item x="26"/>
+        <item x="28"/>
+        <item x="27"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="6"/>
+        <item x="37"/>
+        <item x="5"/>
+        <item x="36"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="2"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="150">
+    <i>
+      <x/>
+      <x v="1"/>
+      <x v="3"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+      <x v="16"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+      <x v="107"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="33"/>
+      <x v="59"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="36"/>
+      <x v="44"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="42"/>
+      <x v="63"/>
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="64"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="43"/>
+      <x v="65"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="45"/>
+      <x v="40"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="51"/>
+      <x v="59"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="52"/>
+      <x v="79"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="53"/>
+      <x v="80"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="71"/>
+      <x v="104"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="77"/>
+      <x v="126"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="86"/>
+      <x v="59"/>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="2"/>
+      <x v="4"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="47"/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="109"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+      <x v="46"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="108"/>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
+      <x v="36"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="48"/>
+      <x v="12"/>
+    </i>
+    <i r="2">
+      <x v="110"/>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="34"/>
+      <x v="38"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="49"/>
+      <x v="15"/>
+    </i>
+    <i r="2">
+      <x v="111"/>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="37"/>
+      <x v="45"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="50"/>
+      <x v="18"/>
+    </i>
+    <i r="2">
+      <x v="112"/>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="40"/>
+      <x v="51"/>
+      <x v="20"/>
+    </i>
+    <i r="2">
+      <x v="61"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="113"/>
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="41"/>
+      <x v="52"/>
+      <x v="22"/>
+    </i>
+    <i r="2">
+      <x v="62"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="114"/>
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="70"/>
+      <x v="53"/>
+      <x v="28"/>
+    </i>
+    <i r="2">
+      <x v="101"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="115"/>
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x v="74"/>
+      <x v="54"/>
+      <x v="30"/>
+    </i>
+    <i r="2">
+      <x v="116"/>
+      <x v="31"/>
+    </i>
+    <i r="2">
+      <x v="119"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="76"/>
+      <x v="55"/>
+      <x v="32"/>
+    </i>
+    <i r="2">
+      <x v="117"/>
+      <x v="33"/>
+    </i>
+    <i r="2">
+      <x v="125"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="87"/>
+      <x v="56"/>
+      <x v="38"/>
+    </i>
+    <i r="2">
+      <x v="118"/>
+      <x v="39"/>
+    </i>
+    <i r="2">
+      <x v="134"/>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="3"/>
+      <x v="18"/>
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="98"/>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+      <x v="5"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="66"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+      <x v="12"/>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+      <x v="29"/>
+      <x v="17"/>
+    </i>
+    <i r="2">
+      <x v="30"/>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="35"/>
+      <x v="39"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="103"/>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+      <x v="17"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="120"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+      <x v="10"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="60"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="62"/>
+      <x v="92"/>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="12"/>
+      <x v="21"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+      <x v="26"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+      <x v="34"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="35"/>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="56"/>
+      <x v="82"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="83"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="57"/>
+      <x v="84"/>
+      <x v="26"/>
+    </i>
+    <i r="2">
+      <x v="85"/>
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="58"/>
+      <x v="90"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="91"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="59"/>
+      <x v="86"/>
+      <x v="9"/>
+    </i>
+    <i r="2">
+      <x v="87"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="60"/>
+      <x v="88"/>
+      <x v="26"/>
+    </i>
+    <i r="2">
+      <x v="89"/>
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="61"/>
+      <x v="27"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="28"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="63"/>
+      <x v="93"/>
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="94"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="80"/>
+      <x v="6"/>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="46"/>
+      <x v="41"/>
+      <x v="24"/>
+    </i>
+    <i r="3">
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="73"/>
+      <x v="43"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="76"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="75"/>
+      <x v="71"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="73"/>
+      <x v="36"/>
+    </i>
+    <i r="2">
+      <x v="75"/>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="4"/>
+      <x v="13"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="67"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="67"/>
+      <x v="14"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="68"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="68"/>
+      <x v="15"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="69"/>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="16"/>
+      <x v="25"/>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+      <x v="121"/>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="39"/>
+      <x v="7"/>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="51"/>
+      <x v="77"/>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="55"/>
+      <x v="81"/>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="69"/>
+      <x v="42"/>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="13"/>
+      <x v="2"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="37"/>
+      <x v="34"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+      <x v="19"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="122"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+      <x v="102"/>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+      <x v="128"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="129"/>
+      <x/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="7"/>
+      <x v="107"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="121"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+      <x v="99"/>
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="100"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+      <x v="33"/>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+      <x v="106"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="31"/>
+      <x v="107"/>
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="121"/>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="32"/>
+      <x v="9"/>
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="78"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="38"/>
+      <x v="57"/>
+      <x v="24"/>
+    </i>
+    <i r="2">
+      <x v="58"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="48"/>
+      <x v="107"/>
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="121"/>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="49"/>
+      <x v="9"/>
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="78"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="50"/>
+      <x v="20"/>
+      <x v="3"/>
+    </i>
+    <i r="2">
+      <x v="123"/>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="54"/>
+      <x v="22"/>
+      <x v="14"/>
+    </i>
+    <i r="2">
+      <x v="31"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="85"/>
+      <x v="133"/>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="8"/>
+      <x v="8"/>
+      <x v="34"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+      <x v="72"/>
+      <x v="34"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+      <x v="23"/>
+      <x v="34"/>
+    </i>
+    <i r="1">
+      <x v="79"/>
+      <x v="130"/>
+      <x v="35"/>
+    </i>
+    <i r="1">
+      <x v="82"/>
+      <x/>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="11"/>
+      <x v="6"/>
+      <x v="7"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+      <x v="11"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+      <x v="74"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+      <x v="24"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+      <x v="32"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="44"/>
+      <x v="70"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="47"/>
+      <x v="7"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="64"/>
+      <x v="96"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="65"/>
+      <x v="95"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="66"/>
+      <x v="97"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="72"/>
+      <x v="105"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="78"/>
+      <x v="127"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="79"/>
+      <x v="131"/>
+      <x v="37"/>
+    </i>
+    <i r="1">
+      <x v="81"/>
+      <x v="7"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="82"/>
+      <x v="1"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="83"/>
+      <x v="124"/>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="84"/>
+      <x v="132"/>
+      <x v="36"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2146,11 +4995,1567 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C582FD-4165-4560-B76F-BC16F261F391}">
+  <dimension ref="A4:D154"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36:J36"/>
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" dimension="3" start="31" min="31" max="32" activeRow="35" activeCol="3" previousRow="35" previousCol="3" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4" count="1">
+              <x v="21"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotSelection>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>246</v>
+      </c>
+      <c r="B20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C20" t="s">
+        <v>334</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>336</v>
+      </c>
+      <c r="D21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>339</v>
+      </c>
+      <c r="D22" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>256</v>
+      </c>
+      <c r="C23" t="s">
+        <v>257</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>288</v>
+      </c>
+      <c r="C25" t="s">
+        <v>289</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>291</v>
+      </c>
+      <c r="D26" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>294</v>
+      </c>
+      <c r="D27" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>279</v>
+      </c>
+      <c r="C28" t="s">
+        <v>280</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>282</v>
+      </c>
+      <c r="D29" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>285</v>
+      </c>
+      <c r="D30" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>306</v>
+      </c>
+      <c r="C31" t="s">
+        <v>307</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>309</v>
+      </c>
+      <c r="D32" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>312</v>
+      </c>
+      <c r="D33" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>247</v>
+      </c>
+      <c r="C34" t="s">
+        <v>250</v>
+      </c>
+      <c r="D34" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>248</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>253</v>
+      </c>
+      <c r="D36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>324</v>
+      </c>
+      <c r="C37" t="s">
+        <v>327</v>
+      </c>
+      <c r="D37" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>325</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>330</v>
+      </c>
+      <c r="D39" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>297</v>
+      </c>
+      <c r="C40" t="s">
+        <v>300</v>
+      </c>
+      <c r="D40" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>298</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>303</v>
+      </c>
+      <c r="D42" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>270</v>
+      </c>
+      <c r="C43" t="s">
+        <v>273</v>
+      </c>
+      <c r="D43" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>276</v>
+      </c>
+      <c r="D44" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>271</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>261</v>
+      </c>
+      <c r="C46" t="s">
+        <v>264</v>
+      </c>
+      <c r="D46" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>267</v>
+      </c>
+      <c r="D47" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>262</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>315</v>
+      </c>
+      <c r="C49" t="s">
+        <v>318</v>
+      </c>
+      <c r="D49" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>321</v>
+      </c>
+      <c r="D50" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>316</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" t="s">
+        <v>153</v>
+      </c>
+      <c r="D57" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>148</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>216</v>
+      </c>
+      <c r="B61" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" t="s">
+        <v>223</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>221</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>225</v>
+      </c>
+      <c r="C63" t="s">
+        <v>226</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>228</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" t="s">
+        <v>218</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>167</v>
+      </c>
+      <c r="B66" t="s">
+        <v>181</v>
+      </c>
+      <c r="C66" t="s">
+        <v>181</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>183</v>
+      </c>
+      <c r="C67" t="s">
+        <v>184</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" t="s">
+        <v>179</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>177</v>
+      </c>
+      <c r="D69" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" t="s">
+        <v>199</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>197</v>
+      </c>
+      <c r="D71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>206</v>
+      </c>
+      <c r="C72" t="s">
+        <v>209</v>
+      </c>
+      <c r="D72" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>207</v>
+      </c>
+      <c r="D73" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>191</v>
+      </c>
+      <c r="C74" t="s">
+        <v>194</v>
+      </c>
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>192</v>
+      </c>
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>186</v>
+      </c>
+      <c r="C76" t="s">
+        <v>187</v>
+      </c>
+      <c r="D76" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>189</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>201</v>
+      </c>
+      <c r="C78" t="s">
+        <v>204</v>
+      </c>
+      <c r="D78" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>202</v>
+      </c>
+      <c r="D79" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>211</v>
+      </c>
+      <c r="C80" t="s">
+        <v>212</v>
+      </c>
+      <c r="D80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>214</v>
+      </c>
+      <c r="D81" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D82" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>169</v>
+      </c>
+      <c r="D83" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" t="s">
+        <v>174</v>
+      </c>
+      <c r="D84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>230</v>
+      </c>
+      <c r="B85" t="s">
+        <v>232</v>
+      </c>
+      <c r="C85" t="s">
+        <v>243</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>238</v>
+      </c>
+      <c r="C87" t="s">
+        <v>239</v>
+      </c>
+      <c r="D87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>241</v>
+      </c>
+      <c r="D88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>231</v>
+      </c>
+      <c r="C89" t="s">
+        <v>232</v>
+      </c>
+      <c r="D89" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>236</v>
+      </c>
+      <c r="D90" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>234</v>
+      </c>
+      <c r="D91" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>390</v>
+      </c>
+      <c r="B92" t="s">
+        <v>391</v>
+      </c>
+      <c r="C92" t="s">
+        <v>392</v>
+      </c>
+      <c r="D92" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>394</v>
+      </c>
+      <c r="D93" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>401</v>
+      </c>
+      <c r="C94" t="s">
+        <v>402</v>
+      </c>
+      <c r="D94" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>404</v>
+      </c>
+      <c r="D95" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>396</v>
+      </c>
+      <c r="C96" t="s">
+        <v>397</v>
+      </c>
+      <c r="D96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>399</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>128</v>
+      </c>
+      <c r="B98" t="s">
+        <v>141</v>
+      </c>
+      <c r="C98" t="s">
+        <v>142</v>
+      </c>
+      <c r="D98" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>113</v>
+      </c>
+      <c r="C99" t="s">
+        <v>131</v>
+      </c>
+      <c r="D99" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>133</v>
+      </c>
+      <c r="C100" t="s">
+        <v>58</v>
+      </c>
+      <c r="D100" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>110</v>
+      </c>
+      <c r="C101" t="s">
+        <v>129</v>
+      </c>
+      <c r="D101" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>138</v>
+      </c>
+      <c r="C102" t="s">
+        <v>139</v>
+      </c>
+      <c r="D102" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>135</v>
+      </c>
+      <c r="C103" t="s">
+        <v>136</v>
+      </c>
+      <c r="D103" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" t="s">
+        <v>14</v>
+      </c>
+      <c r="C104" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>17</v>
+      </c>
+      <c r="D105" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D107" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>19</v>
+      </c>
+      <c r="C108" t="s">
+        <v>20</v>
+      </c>
+      <c r="D108" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>342</v>
+      </c>
+      <c r="B111" t="s">
+        <v>365</v>
+      </c>
+      <c r="C111" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>131</v>
+      </c>
+      <c r="D112" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>376</v>
+      </c>
+      <c r="C113" t="s">
+        <v>379</v>
+      </c>
+      <c r="D113" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>377</v>
+      </c>
+      <c r="D114" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>381</v>
+      </c>
+      <c r="C115" t="s">
+        <v>382</v>
+      </c>
+      <c r="D115" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>373</v>
+      </c>
+      <c r="C116" t="s">
+        <v>374</v>
+      </c>
+      <c r="D116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>350</v>
+      </c>
+      <c r="C117" t="s">
+        <v>114</v>
+      </c>
+      <c r="D117" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>131</v>
+      </c>
+      <c r="D118" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>354</v>
+      </c>
+      <c r="C119" t="s">
+        <v>344</v>
+      </c>
+      <c r="D119" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>346</v>
+      </c>
+      <c r="D120" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>385</v>
+      </c>
+      <c r="C121" t="s">
+        <v>386</v>
+      </c>
+      <c r="D121" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>388</v>
+      </c>
+      <c r="D122" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>348</v>
+      </c>
+      <c r="C123" t="s">
+        <v>114</v>
+      </c>
+      <c r="D123" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>131</v>
+      </c>
+      <c r="D124" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>343</v>
+      </c>
+      <c r="C125" t="s">
+        <v>344</v>
+      </c>
+      <c r="D125" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>346</v>
+      </c>
+      <c r="D126" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>360</v>
+      </c>
+      <c r="C127" t="s">
+        <v>361</v>
+      </c>
+      <c r="D127" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>363</v>
+      </c>
+      <c r="D128" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>368</v>
+      </c>
+      <c r="C129" t="s">
+        <v>371</v>
+      </c>
+      <c r="D129" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
+        <v>369</v>
+      </c>
+      <c r="D130" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>357</v>
+      </c>
+      <c r="C131" t="s">
+        <v>358</v>
+      </c>
+      <c r="D131" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>6</v>
+      </c>
+      <c r="B132" t="s">
+        <v>76</v>
+      </c>
+      <c r="C132" t="s">
+        <v>77</v>
+      </c>
+      <c r="D132" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>54</v>
+      </c>
+      <c r="C133" t="s">
+        <v>79</v>
+      </c>
+      <c r="D133" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>64</v>
+      </c>
+      <c r="C134" t="s">
+        <v>81</v>
+      </c>
+      <c r="D134" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>23</v>
+      </c>
+      <c r="C135" t="s">
+        <v>73</v>
+      </c>
+      <c r="D135" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>67</v>
+      </c>
+      <c r="C136" t="s">
+        <v>83</v>
+      </c>
+      <c r="D136" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>2</v>
+      </c>
+      <c r="B137" t="s">
+        <v>57</v>
+      </c>
+      <c r="C137" t="s">
+        <v>58</v>
+      </c>
+      <c r="D137" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>27</v>
+      </c>
+      <c r="C138" t="s">
+        <v>28</v>
+      </c>
+      <c r="D138" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>54</v>
+      </c>
+      <c r="C139" t="s">
+        <v>55</v>
+      </c>
+      <c r="D139" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>64</v>
+      </c>
+      <c r="C140" t="s">
+        <v>65</v>
+      </c>
+      <c r="D140" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>39</v>
+      </c>
+      <c r="C141" t="s">
+        <v>40</v>
+      </c>
+      <c r="D141" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>45</v>
+      </c>
+      <c r="C142" t="s">
+        <v>46</v>
+      </c>
+      <c r="D142" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>60</v>
+      </c>
+      <c r="C143" t="s">
+        <v>58</v>
+      </c>
+      <c r="D143" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>33</v>
+      </c>
+      <c r="C144" t="s">
+        <v>34</v>
+      </c>
+      <c r="D144" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>70</v>
+      </c>
+      <c r="C145" t="s">
+        <v>71</v>
+      </c>
+      <c r="D145" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>30</v>
+      </c>
+      <c r="C146" t="s">
+        <v>31</v>
+      </c>
+      <c r="D146" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>51</v>
+      </c>
+      <c r="C147" t="s">
+        <v>52</v>
+      </c>
+      <c r="D147" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>48</v>
+      </c>
+      <c r="C148" t="s">
+        <v>49</v>
+      </c>
+      <c r="D148" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>23</v>
+      </c>
+      <c r="C149" t="s">
+        <v>24</v>
+      </c>
+      <c r="D149" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>62</v>
+      </c>
+      <c r="C150" t="s">
+        <v>58</v>
+      </c>
+      <c r="D150" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>67</v>
+      </c>
+      <c r="C151" t="s">
+        <v>68</v>
+      </c>
+      <c r="D151" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>36</v>
+      </c>
+      <c r="C152" t="s">
+        <v>37</v>
+      </c>
+      <c r="D152" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>42</v>
+      </c>
+      <c r="C153" t="s">
+        <v>43</v>
+      </c>
+      <c r="D153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>419</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H150"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B150"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,7 +6566,8 @@
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6073,12 +10479,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7347,7 +11753,7 @@
         <v>70</v>
       </c>
       <c r="D67" t="b">
-        <f t="shared" ref="D67:D95" si="3">EXACT(A67,E67)</f>
+        <f t="shared" ref="D67:D89" si="3">EXACT(A67,E67)</f>
         <v>1</v>
       </c>
       <c r="E67" t="s">
@@ -7424,10 +11830,10 @@
       </c>
       <c r="D71" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>135</v>
+        <v>415</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>